<commit_message>
Up to date and included season leaders.
</commit_message>
<xml_diff>
--- a/AucklandUnitedShots2023-24.xlsx
+++ b/AucklandUnitedShots2023-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukec\Expected Goals Model\ExpectedGoalsModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87419A1B-92C4-48D6-B550-7F98C66A19F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349DD1F6-7178-4530-A187-76AC2B2545A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="694" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="694" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AUFC" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="70">
   <si>
     <t>Outcome</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t xml:space="preserve"> offGoal</t>
+  </si>
+  <si>
+    <t>Suburbs</t>
+  </si>
+  <si>
+    <t>2NL</t>
   </si>
 </sst>
 </file>
@@ -6272,10 +6278,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB4B138-7ACD-493B-86CF-0C45609B4BC0}">
-  <dimension ref="A1:N936"/>
+  <dimension ref="A1:N959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A902" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A937" sqref="A937"/>
+    <sheetView tabSelected="1" topLeftCell="A899" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U918" sqref="U918"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32953,11 +32959,11 @@
         <v>42.5</v>
       </c>
       <c r="F805">
-        <f t="shared" ref="F805:F936" si="59">ABS(E805-40)</f>
+        <f t="shared" ref="F805:F915" si="59">ABS(E805-40)</f>
         <v>2.5</v>
       </c>
       <c r="G805">
-        <f t="shared" ref="G805:G936" si="60">SQRT((120-D805)^2+F805^2)</f>
+        <f t="shared" ref="G805:G915" si="60">SQRT((120-D805)^2+F805^2)</f>
         <v>35.78742796010912</v>
       </c>
       <c r="H805">
@@ -32990,7 +32996,7 @@
         <v>51.214939226752975</v>
       </c>
       <c r="H806">
-        <f t="shared" ref="H806:H936" si="61">IF(A806="goal", 1, 0)</f>
+        <f t="shared" ref="H806:H915" si="61">IF(A806="goal", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="I806">
@@ -34784,7 +34790,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="865" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>8</v>
       </c>
@@ -34813,7 +34819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="866" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>10</v>
       </c>
@@ -34845,7 +34851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="867" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>10</v>
       </c>
@@ -34882,8 +34888,11 @@
       <c r="L867" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="868" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N867">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="868" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A868" s="3" t="s">
         <v>10</v>
       </c>
@@ -34920,8 +34929,11 @@
       <c r="L868" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="869" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N868">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="869" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
         <v>11</v>
       </c>
@@ -34958,8 +34970,11 @@
       <c r="L869" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="870" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N869">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="870" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
         <v>10</v>
       </c>
@@ -34996,8 +35011,11 @@
       <c r="L870" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="871" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N870">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="871" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
         <v>10</v>
       </c>
@@ -35034,8 +35052,11 @@
       <c r="L871" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="872" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N871">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="872" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
         <v>11</v>
       </c>
@@ -35072,8 +35093,11 @@
       <c r="L872" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="873" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N872">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="873" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
         <v>10</v>
       </c>
@@ -35110,8 +35134,11 @@
       <c r="L873" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="874" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N873">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="874" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
         <v>10</v>
       </c>
@@ -35148,8 +35175,11 @@
       <c r="L874" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="875" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N874">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="875" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>11</v>
       </c>
@@ -35186,8 +35216,11 @@
       <c r="L875" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="876" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N875">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="876" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
         <v>9</v>
       </c>
@@ -35224,8 +35257,11 @@
       <c r="L876" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="877" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N876">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="877" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
         <v>11</v>
       </c>
@@ -35260,7 +35296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="878" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
         <v>9</v>
       </c>
@@ -35295,7 +35331,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="879" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
         <v>10</v>
       </c>
@@ -35330,7 +35366,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="880" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
         <v>8</v>
       </c>
@@ -35472,6 +35508,9 @@
       <c r="L883" t="s">
         <v>35</v>
       </c>
+      <c r="N883">
+        <v>9</v>
+      </c>
     </row>
     <row r="884" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
@@ -35510,6 +35549,9 @@
       <c r="L884" t="s">
         <v>35</v>
       </c>
+      <c r="N884">
+        <v>9</v>
+      </c>
     </row>
     <row r="885" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
@@ -35659,6 +35701,9 @@
       <c r="L888" t="s">
         <v>35</v>
       </c>
+      <c r="N888">
+        <v>19</v>
+      </c>
     </row>
     <row r="889" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
@@ -35697,6 +35742,9 @@
       <c r="L889" t="s">
         <v>35</v>
       </c>
+      <c r="N889">
+        <v>9</v>
+      </c>
     </row>
     <row r="890" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
@@ -35735,6 +35783,9 @@
       <c r="L890" t="s">
         <v>35</v>
       </c>
+      <c r="N890">
+        <v>20</v>
+      </c>
     </row>
     <row r="891" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
@@ -35773,6 +35824,9 @@
       <c r="L891" t="s">
         <v>35</v>
       </c>
+      <c r="N891">
+        <v>11</v>
+      </c>
     </row>
     <row r="892" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
@@ -35811,10 +35865,13 @@
       <c r="L892" t="s">
         <v>35</v>
       </c>
+      <c r="N892">
+        <v>7</v>
+      </c>
     </row>
     <row r="893" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B893" t="s">
         <v>59</v>
@@ -35823,18 +35880,18 @@
         <v>59</v>
       </c>
       <c r="D893">
-        <v>106.42</v>
+        <v>111.92</v>
       </c>
       <c r="E893">
-        <v>32.54</v>
+        <v>29.35</v>
       </c>
       <c r="F893">
         <f t="shared" si="59"/>
-        <v>7.4600000000000009</v>
+        <v>10.649999999999999</v>
       </c>
       <c r="G893">
         <f t="shared" si="60"/>
-        <v>15.49412791995729</v>
+        <v>13.368204815905536</v>
       </c>
       <c r="H893">
         <f t="shared" si="61"/>
@@ -35844,15 +35901,18 @@
         <v>9</v>
       </c>
       <c r="J893" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L893" t="s">
         <v>33</v>
       </c>
+      <c r="N893">
+        <v>7</v>
+      </c>
     </row>
     <row r="894" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B894" t="s">
         <v>59</v>
@@ -35861,33 +35921,39 @@
         <v>59</v>
       </c>
       <c r="D894">
-        <v>103.22</v>
+        <v>98.42</v>
       </c>
       <c r="E894">
-        <v>39.119999999999997</v>
+        <v>49.06</v>
       </c>
       <c r="F894">
         <f t="shared" si="59"/>
-        <v>0.88000000000000256</v>
+        <v>9.0600000000000023</v>
       </c>
       <c r="G894">
         <f t="shared" si="60"/>
-        <v>16.803059245268408</v>
+        <v>23.404700382615452</v>
       </c>
       <c r="H894">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I894">
+        <v>17</v>
       </c>
       <c r="J894" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L894" t="s">
         <v>33</v>
       </c>
+      <c r="N894">
+        <v>8</v>
+      </c>
     </row>
     <row r="895" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B895" t="s">
         <v>59</v>
@@ -35896,39 +35962,39 @@
         <v>59</v>
       </c>
       <c r="D895">
-        <v>112.81</v>
+        <v>103.57</v>
       </c>
       <c r="E895">
-        <v>33.97</v>
+        <v>24.37</v>
       </c>
       <c r="F895">
         <f t="shared" si="59"/>
-        <v>6.0300000000000011</v>
+        <v>15.629999999999999</v>
       </c>
       <c r="G895">
         <f t="shared" si="60"/>
-        <v>9.3838691380474817</v>
+        <v>22.676900140892279</v>
       </c>
       <c r="H895">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I895">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J895" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L895" t="s">
         <v>33</v>
       </c>
       <c r="N895">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="896" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B896" t="s">
         <v>59</v>
@@ -35937,33 +36003,39 @@
         <v>59</v>
       </c>
       <c r="D896">
-        <v>104.28</v>
+        <v>97.53</v>
       </c>
       <c r="E896">
-        <v>19.93</v>
+        <v>44.45</v>
       </c>
       <c r="F896">
         <f t="shared" si="59"/>
-        <v>20.07</v>
+        <v>4.4500000000000028</v>
       </c>
       <c r="G896">
         <f t="shared" si="60"/>
-        <v>25.493593312830576</v>
+        <v>22.906405217755143</v>
       </c>
       <c r="H896">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
+      <c r="I896">
+        <v>10</v>
+      </c>
       <c r="J896" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L896" t="s">
         <v>33</v>
       </c>
+      <c r="N896">
+        <v>9</v>
+      </c>
     </row>
     <row r="897" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="B897" t="s">
         <v>59</v>
@@ -35972,35 +36044,29 @@
         <v>59</v>
       </c>
       <c r="D897">
-        <v>112.1</v>
+        <v>106.77</v>
       </c>
       <c r="E897">
-        <v>51.02</v>
+        <v>35.21</v>
       </c>
       <c r="F897">
         <f t="shared" si="59"/>
-        <v>11.020000000000003</v>
+        <v>4.7899999999999991</v>
       </c>
       <c r="G897">
         <f t="shared" si="60"/>
-        <v>13.559144515787128</v>
+        <v>14.070429986322383</v>
       </c>
       <c r="H897">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I897">
-        <v>11</v>
-      </c>
       <c r="J897" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L897" t="s">
         <v>33</v>
       </c>
-      <c r="N897">
-        <v>15</v>
-      </c>
     </row>
     <row r="898" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
@@ -36013,36 +36079,39 @@
         <v>59</v>
       </c>
       <c r="D898">
-        <v>93.27</v>
+        <v>112.45</v>
       </c>
       <c r="E898">
-        <v>45.69</v>
+        <v>52.62</v>
       </c>
       <c r="F898">
         <f t="shared" si="59"/>
-        <v>5.6899999999999977</v>
+        <v>12.619999999999997</v>
       </c>
       <c r="G898">
         <f t="shared" si="60"/>
-        <v>27.328904112678945</v>
+        <v>14.706015775865328</v>
       </c>
       <c r="H898">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="I898">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J898" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L898" t="s">
         <v>33</v>
       </c>
+      <c r="N898">
+        <v>17</v>
+      </c>
     </row>
     <row r="899" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B899" t="s">
         <v>59</v>
@@ -36051,36 +36120,39 @@
         <v>59</v>
       </c>
       <c r="D899">
-        <v>104.11</v>
+        <v>109.97</v>
       </c>
       <c r="E899">
-        <v>33.61</v>
+        <v>38.409999999999997</v>
       </c>
       <c r="F899">
         <f t="shared" si="59"/>
-        <v>6.3900000000000006</v>
+        <v>1.5900000000000034</v>
       </c>
       <c r="G899">
         <f t="shared" si="60"/>
-        <v>17.126710133589579</v>
+        <v>10.155244950270774</v>
       </c>
       <c r="H899">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I899">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J899" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L899" t="s">
         <v>33</v>
       </c>
+      <c r="N899">
+        <v>8</v>
+      </c>
     </row>
     <row r="900" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B900" t="s">
         <v>59</v>
@@ -36089,39 +36161,39 @@
         <v>59</v>
       </c>
       <c r="D900">
-        <v>91.32</v>
+        <v>103.93</v>
       </c>
       <c r="E900">
-        <v>52.26</v>
+        <v>29.35</v>
       </c>
       <c r="F900">
         <f t="shared" si="59"/>
-        <v>12.259999999999998</v>
+        <v>10.649999999999999</v>
       </c>
       <c r="G900">
         <f t="shared" si="60"/>
-        <v>31.190543438677057</v>
+        <v>19.278677340523124</v>
       </c>
       <c r="H900">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I900">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J900" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L900" t="s">
         <v>33</v>
       </c>
       <c r="N900">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="901" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B901" t="s">
         <v>59</v>
@@ -36130,39 +36202,33 @@
         <v>59</v>
       </c>
       <c r="D901">
-        <v>108.9</v>
+        <v>94.87</v>
       </c>
       <c r="E901">
-        <v>40.89</v>
+        <v>31.83</v>
       </c>
       <c r="F901">
         <f t="shared" si="59"/>
-        <v>0.89000000000000057</v>
+        <v>8.1700000000000017</v>
       </c>
       <c r="G901">
         <f t="shared" si="60"/>
-        <v>11.135623018044383</v>
+        <v>26.424719487631268</v>
       </c>
       <c r="H901">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I901">
-        <v>8</v>
-      </c>
       <c r="J901" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L901" t="s">
         <v>33</v>
       </c>
-      <c r="N901">
-        <v>10</v>
-      </c>
     </row>
     <row r="902" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B902" t="s">
         <v>59</v>
@@ -36171,39 +36237,39 @@
         <v>59</v>
       </c>
       <c r="D902">
-        <v>115.3</v>
+        <v>101.26</v>
       </c>
       <c r="E902">
-        <v>37.340000000000003</v>
+        <v>34.32</v>
       </c>
       <c r="F902">
         <f t="shared" si="59"/>
-        <v>2.6599999999999966</v>
+        <v>5.68</v>
       </c>
       <c r="G902">
         <f t="shared" si="60"/>
-        <v>5.4005184936263309</v>
+        <v>19.581879378650044</v>
       </c>
       <c r="H902">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I902">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J902" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L902" t="s">
         <v>33</v>
       </c>
       <c r="N902">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="903" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B903" t="s">
         <v>59</v>
@@ -36212,33 +36278,39 @@
         <v>59</v>
       </c>
       <c r="D903">
-        <v>96.65</v>
+        <v>94.51</v>
       </c>
       <c r="E903">
-        <v>45.16</v>
+        <v>48.18</v>
       </c>
       <c r="F903">
         <f t="shared" si="59"/>
-        <v>5.1599999999999966</v>
+        <v>8.18</v>
       </c>
       <c r="G903">
         <f t="shared" si="60"/>
-        <v>23.913345646312223</v>
+        <v>26.770366078931378</v>
       </c>
       <c r="H903">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
+      <c r="I903">
+        <v>7</v>
+      </c>
       <c r="J903" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L903" t="s">
         <v>33</v>
       </c>
+      <c r="N903">
+        <v>17</v>
+      </c>
     </row>
     <row r="904" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B904" t="s">
         <v>59</v>
@@ -36247,39 +36319,33 @@
         <v>59</v>
       </c>
       <c r="D904">
-        <v>106.42</v>
+        <v>97.53</v>
       </c>
       <c r="E904">
-        <v>36.81</v>
+        <v>41.78</v>
       </c>
       <c r="F904">
         <f t="shared" si="59"/>
-        <v>3.1899999999999977</v>
+        <v>1.7800000000000011</v>
       </c>
       <c r="G904">
         <f t="shared" si="60"/>
-        <v>13.94964157245626</v>
+        <v>22.540392631895301</v>
       </c>
       <c r="H904">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I904">
-        <v>15</v>
-      </c>
       <c r="J904" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L904" t="s">
         <v>33</v>
       </c>
-      <c r="N904">
-        <v>7</v>
-      </c>
     </row>
     <row r="905" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B905" t="s">
         <v>59</v>
@@ -36288,39 +36354,33 @@
         <v>59</v>
       </c>
       <c r="D905">
-        <v>100.73</v>
+        <v>92.03</v>
       </c>
       <c r="E905">
-        <v>53.15</v>
+        <v>45.33</v>
       </c>
       <c r="F905">
         <f t="shared" si="59"/>
-        <v>13.149999999999999</v>
+        <v>5.3299999999999983</v>
       </c>
       <c r="G905">
         <f t="shared" si="60"/>
-        <v>23.329282029243846</v>
+        <v>28.473317333953204</v>
       </c>
       <c r="H905">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I905">
-        <v>5</v>
-      </c>
       <c r="J905" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L905" t="s">
         <v>33</v>
       </c>
-      <c r="N905">
-        <v>7</v>
-      </c>
     </row>
     <row r="906" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B906" t="s">
         <v>59</v>
@@ -36329,34 +36389,34 @@
         <v>59</v>
       </c>
       <c r="D906">
-        <v>105.7</v>
+        <v>103.22</v>
       </c>
       <c r="E906">
-        <v>41.96</v>
+        <v>41.6</v>
       </c>
       <c r="F906">
         <f t="shared" si="59"/>
-        <v>1.9600000000000009</v>
+        <v>1.6000000000000014</v>
       </c>
       <c r="G906">
         <f t="shared" si="60"/>
-        <v>14.433696685187753</v>
+        <v>16.856108684984207</v>
       </c>
       <c r="H906">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="I906">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J906" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L906" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N906">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="907" spans="1:14" x14ac:dyDescent="0.25">
@@ -36370,39 +36430,33 @@
         <v>59</v>
       </c>
       <c r="D907">
-        <v>101.26</v>
+        <v>106.77</v>
       </c>
       <c r="E907">
-        <v>35.21</v>
+        <v>39.47</v>
       </c>
       <c r="F907">
         <f t="shared" si="59"/>
-        <v>4.7899999999999991</v>
+        <v>0.53000000000000114</v>
       </c>
       <c r="G907">
         <f t="shared" si="60"/>
-        <v>19.342484328544764</v>
+        <v>13.240611768343641</v>
       </c>
       <c r="H907">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I907">
-        <v>18</v>
-      </c>
       <c r="J907" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L907" t="s">
-        <v>33</v>
-      </c>
-      <c r="N907">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="908" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B908" t="s">
         <v>59</v>
@@ -36411,36 +36465,33 @@
         <v>59</v>
       </c>
       <c r="D908">
-        <v>99.84</v>
+        <v>93.45</v>
       </c>
       <c r="E908">
-        <v>27.04</v>
+        <v>43.02</v>
       </c>
       <c r="F908">
         <f t="shared" si="59"/>
-        <v>12.96</v>
+        <v>3.0200000000000031</v>
       </c>
       <c r="G908">
         <f t="shared" si="60"/>
-        <v>23.966376447014259</v>
+        <v>26.721206933819435</v>
       </c>
       <c r="H908">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I908">
-        <v>11</v>
-      </c>
       <c r="J908" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L908" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="909" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B909" t="s">
         <v>59</v>
@@ -36449,39 +36500,33 @@
         <v>59</v>
       </c>
       <c r="D909">
-        <v>109.61</v>
+        <v>95.76</v>
       </c>
       <c r="E909">
-        <v>26.68</v>
+        <v>44.8</v>
       </c>
       <c r="F909">
         <f t="shared" si="59"/>
-        <v>13.32</v>
+        <v>4.7999999999999972</v>
       </c>
       <c r="G909">
         <f t="shared" si="60"/>
-        <v>16.893031107530703</v>
+        <v>24.710677853915698</v>
       </c>
       <c r="H909">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I909">
-        <v>10</v>
-      </c>
       <c r="J909" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L909" t="s">
-        <v>33</v>
-      </c>
-      <c r="N909">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="910" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B910" t="s">
         <v>59</v>
@@ -36490,34 +36535,34 @@
         <v>59</v>
       </c>
       <c r="D910">
-        <v>97</v>
+        <v>104.99</v>
       </c>
       <c r="E910">
-        <v>34.14</v>
+        <v>20.64</v>
       </c>
       <c r="F910">
         <f t="shared" si="59"/>
-        <v>5.8599999999999994</v>
+        <v>19.36</v>
       </c>
       <c r="G910">
         <f t="shared" si="60"/>
-        <v>23.734776173370584</v>
+        <v>24.497136567362322</v>
       </c>
       <c r="H910">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I910">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J910" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L910" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N910">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="911" spans="1:14" x14ac:dyDescent="0.25">
@@ -36531,28 +36576,34 @@
         <v>59</v>
       </c>
       <c r="D911">
-        <v>105.53</v>
+        <v>109.08</v>
       </c>
       <c r="E911">
-        <v>54.39</v>
+        <v>30.59</v>
       </c>
       <c r="F911">
         <f t="shared" si="59"/>
-        <v>14.39</v>
+        <v>9.41</v>
       </c>
       <c r="G911">
         <f t="shared" si="60"/>
-        <v>20.407180108971449</v>
+        <v>14.41507891064076</v>
       </c>
       <c r="H911">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
+      <c r="I911">
+        <v>9</v>
+      </c>
       <c r="J911" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L911" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="N911">
+        <v>7</v>
       </c>
     </row>
     <row r="912" spans="1:14" x14ac:dyDescent="0.25">
@@ -36566,34 +36617,28 @@
         <v>59</v>
       </c>
       <c r="D912">
-        <v>98.07</v>
+        <v>96.65</v>
       </c>
       <c r="E912">
-        <v>18.510000000000002</v>
+        <v>29.88</v>
       </c>
       <c r="F912">
         <f t="shared" si="59"/>
-        <v>21.49</v>
+        <v>10.120000000000001</v>
       </c>
       <c r="G912">
         <f t="shared" si="60"/>
-        <v>30.704152813585335</v>
+        <v>25.448711165793835</v>
       </c>
       <c r="H912">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I912">
-        <v>8</v>
-      </c>
       <c r="J912" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L912" t="s">
-        <v>33</v>
-      </c>
-      <c r="N912">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="913" spans="1:14" x14ac:dyDescent="0.25">
@@ -36607,39 +36652,39 @@
         <v>59</v>
       </c>
       <c r="D913">
-        <v>106.42</v>
+        <v>105.88</v>
       </c>
       <c r="E913">
-        <v>47.82</v>
+        <v>48.53</v>
       </c>
       <c r="F913">
         <f t="shared" si="59"/>
-        <v>7.82</v>
+        <v>8.5300000000000011</v>
       </c>
       <c r="G913">
         <f t="shared" si="60"/>
-        <v>15.670634958418244</v>
+        <v>16.496523876259513</v>
       </c>
       <c r="H913">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="I913">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J913" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L913" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N913">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="914" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B914" t="s">
         <v>59</v>
@@ -36648,39 +36693,33 @@
         <v>59</v>
       </c>
       <c r="D914">
-        <v>107.13</v>
+        <v>95.22</v>
       </c>
       <c r="E914">
-        <v>44.62</v>
+        <v>42.85</v>
       </c>
       <c r="F914">
         <f t="shared" si="59"/>
-        <v>4.6199999999999974</v>
+        <v>2.8500000000000014</v>
       </c>
       <c r="G914">
         <f t="shared" si="60"/>
-        <v>13.67411057436644</v>
+        <v>24.943353824215382</v>
       </c>
       <c r="H914">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I914">
-        <v>10</v>
-      </c>
       <c r="J914" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L914" t="s">
         <v>35</v>
       </c>
-      <c r="N914">
-        <v>9</v>
-      </c>
     </row>
     <row r="915" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B915" t="s">
         <v>59</v>
@@ -36689,35 +36728,29 @@
         <v>59</v>
       </c>
       <c r="D915">
-        <v>101.26</v>
+        <v>95.76</v>
       </c>
       <c r="E915">
-        <v>27.93</v>
+        <v>50.84</v>
       </c>
       <c r="F915">
         <f t="shared" si="59"/>
-        <v>12.07</v>
+        <v>10.840000000000003</v>
       </c>
       <c r="G915">
         <f t="shared" si="60"/>
-        <v>22.29063704787281</v>
+        <v>26.553402795122132</v>
       </c>
       <c r="H915">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="I915">
-        <v>11</v>
-      </c>
       <c r="J915" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L915" t="s">
         <v>35</v>
       </c>
-      <c r="N915">
-        <v>7</v>
-      </c>
     </row>
     <row r="916" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
@@ -36730,39 +36763,39 @@
         <v>59</v>
       </c>
       <c r="D916">
-        <v>102.15</v>
+        <v>106.42</v>
       </c>
       <c r="E916">
-        <v>33.61</v>
+        <v>32.54</v>
       </c>
       <c r="F916">
-        <f t="shared" si="59"/>
-        <v>6.3900000000000006</v>
+        <f t="shared" ref="F916:F959" si="62">ABS(E916-40)</f>
+        <v>7.4600000000000009</v>
       </c>
       <c r="G916">
-        <f t="shared" si="60"/>
-        <v>18.959287961313311</v>
+        <f t="shared" ref="G916:G959" si="63">SQRT((120-D916)^2+F916^2)</f>
+        <v>15.49412791995729</v>
       </c>
       <c r="H916">
-        <f t="shared" si="61"/>
+        <f t="shared" ref="H916:H959" si="64">IF(A916="goal", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="I916">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J916" t="s">
         <v>65</v>
       </c>
       <c r="L916" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N916">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="917" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A917" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B917" t="s">
         <v>59</v>
@@ -36771,39 +36804,33 @@
         <v>59</v>
       </c>
       <c r="D917">
-        <v>109.97</v>
+        <v>103.22</v>
       </c>
       <c r="E917">
-        <v>37.520000000000003</v>
+        <v>39.119999999999997</v>
       </c>
       <c r="F917">
-        <f t="shared" si="59"/>
-        <v>2.4799999999999969</v>
+        <f t="shared" si="62"/>
+        <v>0.88000000000000256</v>
       </c>
       <c r="G917">
-        <f t="shared" si="60"/>
-        <v>10.332052071103785</v>
+        <f t="shared" si="63"/>
+        <v>16.803059245268408</v>
       </c>
       <c r="H917">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="I917">
-        <v>11</v>
+        <f t="shared" si="64"/>
+        <v>1</v>
       </c>
       <c r="J917" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L917" t="s">
-        <v>35</v>
-      </c>
-      <c r="N917">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="918" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B918" t="s">
         <v>59</v>
@@ -36812,34 +36839,34 @@
         <v>59</v>
       </c>
       <c r="D918">
-        <v>101.44</v>
+        <v>112.81</v>
       </c>
       <c r="E918">
-        <v>51.02</v>
+        <v>33.97</v>
       </c>
       <c r="F918">
-        <f t="shared" si="59"/>
-        <v>11.020000000000003</v>
+        <f t="shared" si="62"/>
+        <v>6.0300000000000011</v>
       </c>
       <c r="G918">
-        <f t="shared" si="60"/>
-        <v>21.58504111647694</v>
+        <f t="shared" si="63"/>
+        <v>9.3838691380474817</v>
       </c>
       <c r="H918">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>1</v>
       </c>
       <c r="I918">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J918" t="s">
         <v>65</v>
       </c>
       <c r="L918" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N918">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="919" spans="1:14" x14ac:dyDescent="0.25">
@@ -36853,39 +36880,33 @@
         <v>59</v>
       </c>
       <c r="D919">
-        <v>116.9</v>
+        <v>104.28</v>
       </c>
       <c r="E919">
-        <v>48.71</v>
+        <v>19.93</v>
       </c>
       <c r="F919">
-        <f t="shared" si="59"/>
-        <v>8.7100000000000009</v>
+        <f t="shared" si="62"/>
+        <v>20.07</v>
       </c>
       <c r="G919">
-        <f t="shared" si="60"/>
-        <v>9.2452203867728322</v>
+        <f t="shared" si="63"/>
+        <v>25.493593312830576</v>
       </c>
       <c r="H919">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="I919">
-        <v>9</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
       </c>
       <c r="J919" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L919" t="s">
-        <v>35</v>
-      </c>
-      <c r="N919">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="920" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B920" t="s">
         <v>59</v>
@@ -36894,34 +36915,34 @@
         <v>59</v>
       </c>
       <c r="D920">
-        <v>93.63</v>
+        <v>112.1</v>
       </c>
       <c r="E920">
-        <v>35.39</v>
+        <v>51.02</v>
       </c>
       <c r="F920">
-        <f t="shared" si="59"/>
-        <v>4.6099999999999994</v>
+        <f t="shared" si="62"/>
+        <v>11.020000000000003</v>
       </c>
       <c r="G920">
-        <f t="shared" si="60"/>
-        <v>26.769927157166496</v>
+        <f t="shared" si="63"/>
+        <v>13.559144515787128</v>
       </c>
       <c r="H920">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I920">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J920" t="s">
         <v>65</v>
       </c>
       <c r="L920" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N920">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="921" spans="1:14" x14ac:dyDescent="0.25">
@@ -36935,39 +36956,39 @@
         <v>59</v>
       </c>
       <c r="D921">
-        <v>97.89</v>
+        <v>93.27</v>
       </c>
       <c r="E921">
-        <v>38.58</v>
+        <v>45.69</v>
       </c>
       <c r="F921">
-        <f t="shared" si="59"/>
-        <v>1.4200000000000017</v>
+        <f t="shared" si="62"/>
+        <v>5.6899999999999977</v>
       </c>
       <c r="G921">
-        <f t="shared" si="60"/>
-        <v>22.155552351498709</v>
+        <f t="shared" si="63"/>
+        <v>27.328904112678945</v>
       </c>
       <c r="H921">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I921">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="J921" t="s">
         <v>65</v>
       </c>
       <c r="L921" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N921">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="922" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B922" t="s">
         <v>59</v>
@@ -36976,39 +36997,36 @@
         <v>59</v>
       </c>
       <c r="D922">
-        <v>108.55</v>
+        <v>104.11</v>
       </c>
       <c r="E922">
-        <v>37.869999999999997</v>
+        <v>33.61</v>
       </c>
       <c r="F922">
-        <f t="shared" si="59"/>
-        <v>2.1300000000000026</v>
+        <f t="shared" si="62"/>
+        <v>6.3900000000000006</v>
       </c>
       <c r="G922">
-        <f t="shared" si="60"/>
-        <v>11.646432930301023</v>
+        <f t="shared" si="63"/>
+        <v>17.126710133589579</v>
       </c>
       <c r="H922">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>1</v>
       </c>
       <c r="I922">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J922" t="s">
         <v>65</v>
       </c>
       <c r="L922" t="s">
-        <v>35</v>
-      </c>
-      <c r="N922">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="923" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B923" t="s">
         <v>59</v>
@@ -37017,31 +37035,31 @@
         <v>59</v>
       </c>
       <c r="D923">
-        <v>115.3</v>
+        <v>91.32</v>
       </c>
       <c r="E923">
-        <v>54.92</v>
+        <v>52.26</v>
       </c>
       <c r="F923">
-        <f t="shared" si="59"/>
-        <v>14.920000000000002</v>
+        <f t="shared" si="62"/>
+        <v>12.259999999999998</v>
       </c>
       <c r="G923">
-        <f t="shared" si="60"/>
-        <v>15.642774689932732</v>
+        <f t="shared" si="63"/>
+        <v>31.190543438677057</v>
       </c>
       <c r="H923">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I923">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J923" t="s">
         <v>65</v>
       </c>
       <c r="L923" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N923">
         <v>8</v>
@@ -37049,7 +37067,7 @@
     </row>
     <row r="924" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B924" t="s">
         <v>59</v>
@@ -37058,39 +37076,39 @@
         <v>59</v>
       </c>
       <c r="D924">
-        <v>101.44</v>
+        <v>108.9</v>
       </c>
       <c r="E924">
-        <v>41.96</v>
+        <v>40.89</v>
       </c>
       <c r="F924">
-        <f t="shared" si="59"/>
-        <v>1.9600000000000009</v>
+        <f t="shared" si="62"/>
+        <v>0.89000000000000057</v>
       </c>
       <c r="G924">
-        <f t="shared" si="60"/>
-        <v>18.663204440824199</v>
+        <f t="shared" si="63"/>
+        <v>11.135623018044383</v>
       </c>
       <c r="H924">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I924">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J924" t="s">
         <v>65</v>
       </c>
       <c r="L924" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N924">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="925" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B925" t="s">
         <v>59</v>
@@ -37099,31 +37117,34 @@
         <v>59</v>
       </c>
       <c r="D925">
-        <v>110.5</v>
+        <v>115.3</v>
       </c>
       <c r="E925">
-        <v>44.27</v>
+        <v>37.340000000000003</v>
       </c>
       <c r="F925">
-        <f t="shared" si="59"/>
-        <v>4.2700000000000031</v>
+        <f t="shared" si="62"/>
+        <v>2.6599999999999966</v>
       </c>
       <c r="G925">
-        <f t="shared" si="60"/>
-        <v>10.41551246938911</v>
+        <f t="shared" si="63"/>
+        <v>5.4005184936263309</v>
       </c>
       <c r="H925">
-        <f t="shared" si="61"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>1</v>
       </c>
       <c r="I925">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J925" t="s">
         <v>65</v>
       </c>
       <c r="L925" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="N925">
+        <v>7</v>
       </c>
     </row>
     <row r="926" spans="1:14" x14ac:dyDescent="0.25">
@@ -37137,33 +37158,33 @@
         <v>59</v>
       </c>
       <c r="D926">
-        <v>87.76</v>
+        <v>96.65</v>
       </c>
       <c r="E926">
-        <v>54.21</v>
+        <v>45.16</v>
       </c>
       <c r="F926">
-        <f t="shared" si="59"/>
-        <v>14.21</v>
+        <f t="shared" si="62"/>
+        <v>5.1599999999999966</v>
       </c>
       <c r="G926">
-        <f t="shared" si="60"/>
-        <v>35.232679432594956</v>
+        <f t="shared" si="63"/>
+        <v>23.913345646312223</v>
       </c>
       <c r="H926">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="J926" t="s">
         <v>66</v>
       </c>
       <c r="L926" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="927" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A927" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B927" t="s">
         <v>59</v>
@@ -37172,36 +37193,39 @@
         <v>59</v>
       </c>
       <c r="D927">
-        <v>100.02</v>
+        <v>106.42</v>
       </c>
       <c r="E927">
-        <v>38.76</v>
+        <v>36.81</v>
       </c>
       <c r="F927">
-        <f t="shared" si="59"/>
-        <v>1.240000000000002</v>
+        <f t="shared" si="62"/>
+        <v>3.1899999999999977</v>
       </c>
       <c r="G927">
-        <f t="shared" si="60"/>
-        <v>20.018441497778994</v>
+        <f t="shared" si="63"/>
+        <v>13.94964157245626</v>
       </c>
       <c r="H927">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I927">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J927" t="s">
         <v>65</v>
       </c>
       <c r="L927" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="N927">
+        <v>7</v>
       </c>
     </row>
     <row r="928" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A928" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B928" t="s">
         <v>59</v>
@@ -37210,39 +37234,39 @@
         <v>59</v>
       </c>
       <c r="D928">
-        <v>98.95</v>
+        <v>100.73</v>
       </c>
       <c r="E928">
-        <v>35.92</v>
+        <v>53.15</v>
       </c>
       <c r="F928">
-        <f t="shared" si="59"/>
-        <v>4.0799999999999983</v>
+        <f t="shared" si="62"/>
+        <v>13.149999999999999</v>
       </c>
       <c r="G928">
-        <f t="shared" si="60"/>
-        <v>21.441755991522708</v>
+        <f t="shared" si="63"/>
+        <v>23.329282029243846</v>
       </c>
       <c r="H928">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I928">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="J928" t="s">
         <v>65</v>
       </c>
       <c r="L928" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N928">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="929" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A929" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B929" t="s">
         <v>59</v>
@@ -37251,34 +37275,34 @@
         <v>59</v>
       </c>
       <c r="D929">
-        <v>117.25</v>
+        <v>105.7</v>
       </c>
       <c r="E929">
-        <v>26.15</v>
+        <v>41.96</v>
       </c>
       <c r="F929">
-        <f t="shared" si="59"/>
-        <v>13.850000000000001</v>
+        <f t="shared" si="62"/>
+        <v>1.9600000000000009</v>
       </c>
       <c r="G929">
-        <f t="shared" si="60"/>
-        <v>14.120375349118735</v>
+        <f t="shared" si="63"/>
+        <v>14.433696685187753</v>
       </c>
       <c r="H929">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I929">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J929" t="s">
         <v>65</v>
       </c>
       <c r="L929" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N929">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="930" spans="1:14" x14ac:dyDescent="0.25">
@@ -37292,39 +37316,39 @@
         <v>59</v>
       </c>
       <c r="D930">
-        <v>102.69</v>
+        <v>101.26</v>
       </c>
       <c r="E930">
-        <v>40.18</v>
+        <v>35.21</v>
       </c>
       <c r="F930">
-        <f t="shared" si="59"/>
-        <v>0.17999999999999972</v>
+        <f t="shared" si="62"/>
+        <v>4.7899999999999991</v>
       </c>
       <c r="G930">
-        <f t="shared" si="60"/>
-        <v>17.310935849918689</v>
+        <f t="shared" si="63"/>
+        <v>19.342484328544764</v>
       </c>
       <c r="H930">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I930">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J930" t="s">
         <v>65</v>
       </c>
       <c r="L930" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N930">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="931" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A931" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B931" t="s">
         <v>59</v>
@@ -37333,39 +37357,39 @@
         <v>59</v>
       </c>
       <c r="D931">
-        <v>104.46</v>
+        <v>99.84</v>
       </c>
       <c r="E931">
-        <v>49.24</v>
+        <v>27.04</v>
       </c>
       <c r="F931">
-        <f t="shared" si="59"/>
-        <v>9.240000000000002</v>
+        <f t="shared" si="62"/>
+        <v>12.96</v>
       </c>
       <c r="G931">
-        <f t="shared" si="60"/>
-        <v>18.079524330025951</v>
+        <f t="shared" si="63"/>
+        <v>23.966376447014259</v>
       </c>
       <c r="H931">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I931">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J931" t="s">
         <v>65</v>
       </c>
       <c r="L931" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N931">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="932" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A932" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B932" t="s">
         <v>59</v>
@@ -37374,34 +37398,34 @@
         <v>59</v>
       </c>
       <c r="D932">
-        <v>102.33</v>
+        <v>109.61</v>
       </c>
       <c r="E932">
-        <v>38.049999999999997</v>
+        <v>26.68</v>
       </c>
       <c r="F932">
-        <f t="shared" si="59"/>
-        <v>1.9500000000000028</v>
+        <f t="shared" si="62"/>
+        <v>13.32</v>
       </c>
       <c r="G932">
-        <f t="shared" si="60"/>
-        <v>17.777272006694393</v>
+        <f t="shared" si="63"/>
+        <v>16.893031107530703</v>
       </c>
       <c r="H932">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I932">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J932" t="s">
         <v>65</v>
       </c>
       <c r="L932" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N932">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="933" spans="1:14" x14ac:dyDescent="0.25">
@@ -37415,39 +37439,39 @@
         <v>59</v>
       </c>
       <c r="D933">
-        <v>115.3</v>
+        <v>97</v>
       </c>
       <c r="E933">
-        <v>41.78</v>
+        <v>34.14</v>
       </c>
       <c r="F933">
-        <f t="shared" si="59"/>
-        <v>1.7800000000000011</v>
+        <f t="shared" si="62"/>
+        <v>5.8599999999999994</v>
       </c>
       <c r="G933">
-        <f t="shared" si="60"/>
-        <v>5.0257735722971075</v>
+        <f t="shared" si="63"/>
+        <v>23.734776173370584</v>
       </c>
       <c r="H933">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I933">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J933" t="s">
         <v>65</v>
       </c>
       <c r="L933" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N933">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="934" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A934" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B934" t="s">
         <v>59</v>
@@ -37456,39 +37480,33 @@
         <v>59</v>
       </c>
       <c r="D934">
-        <v>112.1</v>
+        <v>105.53</v>
       </c>
       <c r="E934">
-        <v>41.43</v>
+        <v>54.39</v>
       </c>
       <c r="F934">
-        <f t="shared" si="59"/>
-        <v>1.4299999999999997</v>
+        <f t="shared" si="62"/>
+        <v>14.39</v>
       </c>
       <c r="G934">
-        <f t="shared" si="60"/>
-        <v>8.0283809077546948</v>
+        <f t="shared" si="63"/>
+        <v>20.407180108971449</v>
       </c>
       <c r="H934">
-        <f t="shared" si="61"/>
-        <v>1</v>
-      </c>
-      <c r="I934">
-        <v>17</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
       </c>
       <c r="J934" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L934" t="s">
-        <v>35</v>
-      </c>
-      <c r="N934">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="935" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A935" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B935" t="s">
         <v>59</v>
@@ -37497,39 +37515,39 @@
         <v>59</v>
       </c>
       <c r="D935">
-        <v>111.92</v>
+        <v>98.07</v>
       </c>
       <c r="E935">
-        <v>22.6</v>
+        <v>18.510000000000002</v>
       </c>
       <c r="F935">
-        <f t="shared" si="59"/>
-        <v>17.399999999999999</v>
+        <f t="shared" si="62"/>
+        <v>21.49</v>
       </c>
       <c r="G935">
-        <f t="shared" si="60"/>
-        <v>19.184535438732937</v>
+        <f t="shared" si="63"/>
+        <v>30.704152813585335</v>
       </c>
       <c r="H935">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I935">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J935" t="s">
         <v>65</v>
       </c>
       <c r="L935" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N935">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="936" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A936" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B936" t="s">
         <v>59</v>
@@ -37538,33 +37556,970 @@
         <v>59</v>
       </c>
       <c r="D936">
-        <v>110.5</v>
+        <v>106.42</v>
       </c>
       <c r="E936">
-        <v>35.39</v>
+        <v>47.82</v>
       </c>
       <c r="F936">
-        <f t="shared" si="59"/>
-        <v>4.6099999999999994</v>
+        <f t="shared" si="62"/>
+        <v>7.82</v>
       </c>
       <c r="G936">
-        <f t="shared" si="60"/>
-        <v>10.559455478385237</v>
+        <f t="shared" si="63"/>
+        <v>15.670634958418244</v>
       </c>
       <c r="H936">
-        <f t="shared" si="61"/>
-        <v>1</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
       </c>
       <c r="I936">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J936" t="s">
         <v>65</v>
       </c>
       <c r="L936" t="s">
+        <v>33</v>
+      </c>
+      <c r="N936">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="937" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>10</v>
+      </c>
+      <c r="B937" t="s">
+        <v>59</v>
+      </c>
+      <c r="C937" t="s">
+        <v>59</v>
+      </c>
+      <c r="D937">
+        <v>107.13</v>
+      </c>
+      <c r="E937">
+        <v>44.62</v>
+      </c>
+      <c r="F937">
+        <f t="shared" si="62"/>
+        <v>4.6199999999999974</v>
+      </c>
+      <c r="G937">
+        <f t="shared" si="63"/>
+        <v>13.67411057436644</v>
+      </c>
+      <c r="H937">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I937">
+        <v>10</v>
+      </c>
+      <c r="J937" t="s">
+        <v>65</v>
+      </c>
+      <c r="L937" t="s">
         <v>35</v>
       </c>
-      <c r="N936">
+      <c r="N937">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="938" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>10</v>
+      </c>
+      <c r="B938" t="s">
+        <v>59</v>
+      </c>
+      <c r="C938" t="s">
+        <v>59</v>
+      </c>
+      <c r="D938">
+        <v>101.26</v>
+      </c>
+      <c r="E938">
+        <v>27.93</v>
+      </c>
+      <c r="F938">
+        <f t="shared" si="62"/>
+        <v>12.07</v>
+      </c>
+      <c r="G938">
+        <f t="shared" si="63"/>
+        <v>22.29063704787281</v>
+      </c>
+      <c r="H938">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I938">
+        <v>11</v>
+      </c>
+      <c r="J938" t="s">
+        <v>65</v>
+      </c>
+      <c r="L938" t="s">
+        <v>35</v>
+      </c>
+      <c r="N938">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="939" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>10</v>
+      </c>
+      <c r="B939" t="s">
+        <v>59</v>
+      </c>
+      <c r="C939" t="s">
+        <v>59</v>
+      </c>
+      <c r="D939">
+        <v>102.15</v>
+      </c>
+      <c r="E939">
+        <v>33.61</v>
+      </c>
+      <c r="F939">
+        <f t="shared" si="62"/>
+        <v>6.3900000000000006</v>
+      </c>
+      <c r="G939">
+        <f t="shared" si="63"/>
+        <v>18.959287961313311</v>
+      </c>
+      <c r="H939">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I939">
+        <v>10</v>
+      </c>
+      <c r="J939" t="s">
+        <v>65</v>
+      </c>
+      <c r="L939" t="s">
+        <v>35</v>
+      </c>
+      <c r="N939">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="940" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>8</v>
+      </c>
+      <c r="B940" t="s">
+        <v>59</v>
+      </c>
+      <c r="C940" t="s">
+        <v>59</v>
+      </c>
+      <c r="D940">
+        <v>109.97</v>
+      </c>
+      <c r="E940">
+        <v>37.520000000000003</v>
+      </c>
+      <c r="F940">
+        <f t="shared" si="62"/>
+        <v>2.4799999999999969</v>
+      </c>
+      <c r="G940">
+        <f t="shared" si="63"/>
+        <v>10.332052071103785</v>
+      </c>
+      <c r="H940">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I940">
+        <v>11</v>
+      </c>
+      <c r="J940" t="s">
+        <v>65</v>
+      </c>
+      <c r="L940" t="s">
+        <v>35</v>
+      </c>
+      <c r="N940">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="941" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>10</v>
+      </c>
+      <c r="B941" t="s">
+        <v>59</v>
+      </c>
+      <c r="C941" t="s">
+        <v>59</v>
+      </c>
+      <c r="D941">
+        <v>101.44</v>
+      </c>
+      <c r="E941">
+        <v>51.02</v>
+      </c>
+      <c r="F941">
+        <f t="shared" si="62"/>
+        <v>11.020000000000003</v>
+      </c>
+      <c r="G941">
+        <f t="shared" si="63"/>
+        <v>21.58504111647694</v>
+      </c>
+      <c r="H941">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I941">
+        <v>15</v>
+      </c>
+      <c r="J941" t="s">
+        <v>65</v>
+      </c>
+      <c r="L941" t="s">
+        <v>35</v>
+      </c>
+      <c r="N941">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="942" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>8</v>
+      </c>
+      <c r="B942" t="s">
+        <v>59</v>
+      </c>
+      <c r="C942" t="s">
+        <v>59</v>
+      </c>
+      <c r="D942">
+        <v>116.9</v>
+      </c>
+      <c r="E942">
+        <v>48.71</v>
+      </c>
+      <c r="F942">
+        <f t="shared" si="62"/>
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="G942">
+        <f t="shared" si="63"/>
+        <v>9.2452203867728322</v>
+      </c>
+      <c r="H942">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I942">
+        <v>9</v>
+      </c>
+      <c r="J942" t="s">
+        <v>65</v>
+      </c>
+      <c r="L942" t="s">
+        <v>35</v>
+      </c>
+      <c r="N942">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="943" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>10</v>
+      </c>
+      <c r="B943" t="s">
+        <v>59</v>
+      </c>
+      <c r="C943" t="s">
+        <v>59</v>
+      </c>
+      <c r="D943">
+        <v>93.63</v>
+      </c>
+      <c r="E943">
+        <v>35.39</v>
+      </c>
+      <c r="F943">
+        <f t="shared" si="62"/>
+        <v>4.6099999999999994</v>
+      </c>
+      <c r="G943">
+        <f t="shared" si="63"/>
+        <v>26.769927157166496</v>
+      </c>
+      <c r="H943">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I943">
+        <v>8</v>
+      </c>
+      <c r="J943" t="s">
+        <v>65</v>
+      </c>
+      <c r="L943" t="s">
+        <v>35</v>
+      </c>
+      <c r="N943">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="944" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A944" t="s">
+        <v>10</v>
+      </c>
+      <c r="B944" t="s">
+        <v>59</v>
+      </c>
+      <c r="C944" t="s">
+        <v>59</v>
+      </c>
+      <c r="D944">
+        <v>97.89</v>
+      </c>
+      <c r="E944">
+        <v>38.58</v>
+      </c>
+      <c r="F944">
+        <f t="shared" si="62"/>
+        <v>1.4200000000000017</v>
+      </c>
+      <c r="G944">
+        <f t="shared" si="63"/>
+        <v>22.155552351498709</v>
+      </c>
+      <c r="H944">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I944">
+        <v>15</v>
+      </c>
+      <c r="J944" t="s">
+        <v>65</v>
+      </c>
+      <c r="L944" t="s">
+        <v>35</v>
+      </c>
+      <c r="N944">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="945" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A945" t="s">
+        <v>10</v>
+      </c>
+      <c r="B945" t="s">
+        <v>59</v>
+      </c>
+      <c r="C945" t="s">
+        <v>59</v>
+      </c>
+      <c r="D945">
+        <v>108.55</v>
+      </c>
+      <c r="E945">
+        <v>37.869999999999997</v>
+      </c>
+      <c r="F945">
+        <f t="shared" si="62"/>
+        <v>2.1300000000000026</v>
+      </c>
+      <c r="G945">
+        <f t="shared" si="63"/>
+        <v>11.646432930301023</v>
+      </c>
+      <c r="H945">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I945">
+        <v>10</v>
+      </c>
+      <c r="J945" t="s">
+        <v>65</v>
+      </c>
+      <c r="L945" t="s">
+        <v>35</v>
+      </c>
+      <c r="N945">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="946" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A946" t="s">
+        <v>10</v>
+      </c>
+      <c r="B946" t="s">
+        <v>59</v>
+      </c>
+      <c r="C946" t="s">
+        <v>59</v>
+      </c>
+      <c r="D946">
+        <v>115.3</v>
+      </c>
+      <c r="E946">
+        <v>54.92</v>
+      </c>
+      <c r="F946">
+        <f t="shared" si="62"/>
+        <v>14.920000000000002</v>
+      </c>
+      <c r="G946">
+        <f t="shared" si="63"/>
+        <v>15.642774689932732</v>
+      </c>
+      <c r="H946">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I946">
+        <v>14</v>
+      </c>
+      <c r="J946" t="s">
+        <v>65</v>
+      </c>
+      <c r="L946" t="s">
+        <v>35</v>
+      </c>
+      <c r="N946">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="947" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A947" t="s">
+        <v>10</v>
+      </c>
+      <c r="B947" t="s">
+        <v>59</v>
+      </c>
+      <c r="C947" t="s">
+        <v>59</v>
+      </c>
+      <c r="D947">
+        <v>101.44</v>
+      </c>
+      <c r="E947">
+        <v>41.96</v>
+      </c>
+      <c r="F947">
+        <f t="shared" si="62"/>
+        <v>1.9600000000000009</v>
+      </c>
+      <c r="G947">
+        <f t="shared" si="63"/>
+        <v>18.663204440824199</v>
+      </c>
+      <c r="H947">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I947">
+        <v>7</v>
+      </c>
+      <c r="J947" t="s">
+        <v>65</v>
+      </c>
+      <c r="L947" t="s">
+        <v>35</v>
+      </c>
+      <c r="N947">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="948" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A948" t="s">
+        <v>10</v>
+      </c>
+      <c r="B948" t="s">
+        <v>59</v>
+      </c>
+      <c r="C948" t="s">
+        <v>59</v>
+      </c>
+      <c r="D948">
+        <v>110.5</v>
+      </c>
+      <c r="E948">
+        <v>44.27</v>
+      </c>
+      <c r="F948">
+        <f t="shared" si="62"/>
+        <v>4.2700000000000031</v>
+      </c>
+      <c r="G948">
+        <f t="shared" si="63"/>
+        <v>10.41551246938911</v>
+      </c>
+      <c r="H948">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I948">
+        <v>14</v>
+      </c>
+      <c r="J948" t="s">
+        <v>65</v>
+      </c>
+      <c r="L948" t="s">
+        <v>35</v>
+      </c>
+      <c r="N948">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="949" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A949" t="s">
+        <v>8</v>
+      </c>
+      <c r="B949" t="s">
+        <v>59</v>
+      </c>
+      <c r="C949" t="s">
+        <v>59</v>
+      </c>
+      <c r="D949">
+        <v>87.76</v>
+      </c>
+      <c r="E949">
+        <v>54.21</v>
+      </c>
+      <c r="F949">
+        <f t="shared" si="62"/>
+        <v>14.21</v>
+      </c>
+      <c r="G949">
+        <f t="shared" si="63"/>
+        <v>35.232679432594956</v>
+      </c>
+      <c r="H949">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="J949" t="s">
+        <v>66</v>
+      </c>
+      <c r="L949" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="950" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A950" t="s">
+        <v>8</v>
+      </c>
+      <c r="B950" t="s">
+        <v>59</v>
+      </c>
+      <c r="C950" t="s">
+        <v>59</v>
+      </c>
+      <c r="D950">
+        <v>100.02</v>
+      </c>
+      <c r="E950">
+        <v>38.76</v>
+      </c>
+      <c r="F950">
+        <f t="shared" si="62"/>
+        <v>1.240000000000002</v>
+      </c>
+      <c r="G950">
+        <f t="shared" si="63"/>
+        <v>20.018441497778994</v>
+      </c>
+      <c r="H950">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I950">
+        <v>9</v>
+      </c>
+      <c r="J950" t="s">
+        <v>65</v>
+      </c>
+      <c r="L950" t="s">
+        <v>35</v>
+      </c>
+      <c r="N950">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="951" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A951" t="s">
+        <v>10</v>
+      </c>
+      <c r="B951" t="s">
+        <v>59</v>
+      </c>
+      <c r="C951" t="s">
+        <v>59</v>
+      </c>
+      <c r="D951">
+        <v>98.95</v>
+      </c>
+      <c r="E951">
+        <v>35.92</v>
+      </c>
+      <c r="F951">
+        <f t="shared" si="62"/>
+        <v>4.0799999999999983</v>
+      </c>
+      <c r="G951">
+        <f t="shared" si="63"/>
+        <v>21.441755991522708</v>
+      </c>
+      <c r="H951">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I951">
+        <v>17</v>
+      </c>
+      <c r="J951" t="s">
+        <v>65</v>
+      </c>
+      <c r="L951" t="s">
+        <v>35</v>
+      </c>
+      <c r="N951">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="952" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A952" t="s">
+        <v>8</v>
+      </c>
+      <c r="B952" t="s">
+        <v>59</v>
+      </c>
+      <c r="C952" t="s">
+        <v>59</v>
+      </c>
+      <c r="D952">
+        <v>117.25</v>
+      </c>
+      <c r="E952">
+        <v>26.15</v>
+      </c>
+      <c r="F952">
+        <f t="shared" si="62"/>
+        <v>13.850000000000001</v>
+      </c>
+      <c r="G952">
+        <f t="shared" si="63"/>
+        <v>14.120375349118735</v>
+      </c>
+      <c r="H952">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I952">
+        <v>19</v>
+      </c>
+      <c r="J952" t="s">
+        <v>65</v>
+      </c>
+      <c r="L952" t="s">
+        <v>35</v>
+      </c>
+      <c r="N952">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="953" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>8</v>
+      </c>
+      <c r="B953" t="s">
+        <v>59</v>
+      </c>
+      <c r="C953" t="s">
+        <v>59</v>
+      </c>
+      <c r="D953">
+        <v>102.69</v>
+      </c>
+      <c r="E953">
+        <v>40.18</v>
+      </c>
+      <c r="F953">
+        <f t="shared" si="62"/>
+        <v>0.17999999999999972</v>
+      </c>
+      <c r="G953">
+        <f t="shared" si="63"/>
+        <v>17.310935849918689</v>
+      </c>
+      <c r="H953">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I953">
+        <v>14</v>
+      </c>
+      <c r="J953" t="s">
+        <v>65</v>
+      </c>
+      <c r="L953" t="s">
+        <v>35</v>
+      </c>
+      <c r="N953">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="954" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A954" t="s">
+        <v>8</v>
+      </c>
+      <c r="B954" t="s">
+        <v>59</v>
+      </c>
+      <c r="C954" t="s">
+        <v>59</v>
+      </c>
+      <c r="D954">
+        <v>104.46</v>
+      </c>
+      <c r="E954">
+        <v>49.24</v>
+      </c>
+      <c r="F954">
+        <f t="shared" si="62"/>
+        <v>9.240000000000002</v>
+      </c>
+      <c r="G954">
+        <f t="shared" si="63"/>
+        <v>18.079524330025951</v>
+      </c>
+      <c r="H954">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I954">
+        <v>9</v>
+      </c>
+      <c r="J954" t="s">
+        <v>65</v>
+      </c>
+      <c r="L954" t="s">
+        <v>35</v>
+      </c>
+      <c r="N954">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="955" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A955" t="s">
+        <v>10</v>
+      </c>
+      <c r="B955" t="s">
+        <v>59</v>
+      </c>
+      <c r="C955" t="s">
+        <v>59</v>
+      </c>
+      <c r="D955">
+        <v>102.33</v>
+      </c>
+      <c r="E955">
+        <v>38.049999999999997</v>
+      </c>
+      <c r="F955">
+        <f t="shared" si="62"/>
+        <v>1.9500000000000028</v>
+      </c>
+      <c r="G955">
+        <f t="shared" si="63"/>
+        <v>17.777272006694393</v>
+      </c>
+      <c r="H955">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I955">
+        <v>8</v>
+      </c>
+      <c r="J955" t="s">
+        <v>65</v>
+      </c>
+      <c r="L955" t="s">
+        <v>35</v>
+      </c>
+      <c r="N955">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="956" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A956" t="s">
+        <v>10</v>
+      </c>
+      <c r="B956" t="s">
+        <v>59</v>
+      </c>
+      <c r="C956" t="s">
+        <v>59</v>
+      </c>
+      <c r="D956">
+        <v>115.3</v>
+      </c>
+      <c r="E956">
+        <v>41.78</v>
+      </c>
+      <c r="F956">
+        <f t="shared" si="62"/>
+        <v>1.7800000000000011</v>
+      </c>
+      <c r="G956">
+        <f t="shared" si="63"/>
+        <v>5.0257735722971075</v>
+      </c>
+      <c r="H956">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I956">
+        <v>9</v>
+      </c>
+      <c r="J956" t="s">
+        <v>65</v>
+      </c>
+      <c r="L956" t="s">
+        <v>35</v>
+      </c>
+      <c r="N956">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="957" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A957" t="s">
+        <v>9</v>
+      </c>
+      <c r="B957" t="s">
+        <v>59</v>
+      </c>
+      <c r="C957" t="s">
+        <v>59</v>
+      </c>
+      <c r="D957">
+        <v>112.1</v>
+      </c>
+      <c r="E957">
+        <v>41.43</v>
+      </c>
+      <c r="F957">
+        <f t="shared" si="62"/>
+        <v>1.4299999999999997</v>
+      </c>
+      <c r="G957">
+        <f t="shared" si="63"/>
+        <v>8.0283809077546948</v>
+      </c>
+      <c r="H957">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="I957">
+        <v>17</v>
+      </c>
+      <c r="J957" t="s">
+        <v>65</v>
+      </c>
+      <c r="L957" t="s">
+        <v>35</v>
+      </c>
+      <c r="N957">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="958" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A958" t="s">
+        <v>10</v>
+      </c>
+      <c r="B958" t="s">
+        <v>59</v>
+      </c>
+      <c r="C958" t="s">
+        <v>59</v>
+      </c>
+      <c r="D958">
+        <v>111.92</v>
+      </c>
+      <c r="E958">
+        <v>22.6</v>
+      </c>
+      <c r="F958">
+        <f t="shared" si="62"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G958">
+        <f t="shared" si="63"/>
+        <v>19.184535438732937</v>
+      </c>
+      <c r="H958">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="I958">
+        <v>19</v>
+      </c>
+      <c r="J958" t="s">
+        <v>65</v>
+      </c>
+      <c r="L958" t="s">
+        <v>35</v>
+      </c>
+      <c r="N958">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="959" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A959" t="s">
+        <v>9</v>
+      </c>
+      <c r="B959" t="s">
+        <v>59</v>
+      </c>
+      <c r="C959" t="s">
+        <v>59</v>
+      </c>
+      <c r="D959">
+        <v>110.5</v>
+      </c>
+      <c r="E959">
+        <v>35.39</v>
+      </c>
+      <c r="F959">
+        <f t="shared" si="62"/>
+        <v>4.6099999999999994</v>
+      </c>
+      <c r="G959">
+        <f t="shared" si="63"/>
+        <v>10.559455478385237</v>
+      </c>
+      <c r="H959">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="I959">
+        <v>17</v>
+      </c>
+      <c r="J959" t="s">
+        <v>65</v>
+      </c>
+      <c r="L959" t="s">
+        <v>35</v>
+      </c>
+      <c r="N959">
         <v>8</v>
       </c>
     </row>

</xml_diff>